<commit_message>
Actualización test estudios advertencias
</commit_message>
<xml_diff>
--- a/bateria_tests/estudios/plantilla_estudios_advertencias.xlsx
+++ b/bateria_tests/estudios/plantilla_estudios_advertencias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\OneDrive\Documentos\Practicas_UOC\datos_muestras\bateria_tests\estudios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4892AE77-6CE2-412F-850D-B7FD37238306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3E7E68-E6F8-4D29-9CFE-61AB3FE50A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="1400" windowWidth="20570" windowHeight="7450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Descripción</t>
   </si>
@@ -57,19 +57,10 @@
     <t>efe</t>
   </si>
   <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>ff</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
     <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
   </si>
   <si>
     <t>aa</t>
@@ -421,7 +412,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -456,59 +447,51 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
+      <c r="D2" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E2" s="3">
+        <v>46752</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3">
+        <v>46752</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>10</v>
+      <c r="D4" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E4" s="3">
+        <v>46752</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
@@ -519,16 +502,13 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="D5" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E5" s="3">
+        <v>46752</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>

</xml_diff>